<commit_message>
spotify data modification in excel sheet format no content was removed.
</commit_message>
<xml_diff>
--- a/Spotify_data (1).xlsx
+++ b/Spotify_data (1).xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A68C3787-B23B-4CF1-914A-ADFBCE93CB4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B66B517-6386-4E59-813A-B360B065BE09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{C02C7CA9-98BC-4463-80C7-53762558B11B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$U$521</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -936,7 +939,7 @@
   <dimension ref="A1:U521"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D526" sqref="D526"/>
+      <selection activeCell="U8" sqref="U8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -960,6 +963,7 @@
     <col min="19" max="19" width="19.5546875" customWidth="1"/>
     <col min="20" max="20" width="8.88671875" customWidth="1"/>
     <col min="21" max="21" width="17.88671875" customWidth="1"/>
+    <col min="22" max="22" width="14.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.3">
@@ -35347,6 +35351,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:U521" xr:uid="{631348B3-AD0C-4320-A243-D3FCC32A56AB}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>